<commit_message>
update complete, cancel genectics case
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -116,6 +116,36 @@
   </si>
   <si>
     <t>CA-R723QKZS</t>
+  </si>
+  <si>
+    <t>CA-7NU4KR4K</t>
+  </si>
+  <si>
+    <t>CA-6GPALHPJ</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>CA-8KC7X7RK</t>
+  </si>
+  <si>
+    <t>CA-DNYHHAIO</t>
+  </si>
+  <si>
+    <t>CA-DFWMFRE9</t>
+  </si>
+  <si>
+    <t>CA-CU2I5L9E</t>
+  </si>
+  <si>
+    <t>CA-BNKDESZ6</t>
+  </si>
+  <si>
+    <t>CA-FR2PHPWO</t>
+  </si>
+  <si>
+    <t>CA-5EDNCJRQ</t>
   </si>
 </sst>
 </file>
@@ -540,7 +570,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>
@@ -637,7 +667,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update genetics denied, logout provider
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>id</t>
   </si>
@@ -146,6 +146,66 @@
   </si>
   <si>
     <t>CA-5EDNCJRQ</t>
+  </si>
+  <si>
+    <t>CA-NN0LBHTF</t>
+  </si>
+  <si>
+    <t>CA-2555KGWB</t>
+  </si>
+  <si>
+    <t>CA-QJPKWCFS</t>
+  </si>
+  <si>
+    <t>CA-J9JRJMAM</t>
+  </si>
+  <si>
+    <t>CA-3U12KDIS</t>
+  </si>
+  <si>
+    <t>CA-J7JBFQ38</t>
+  </si>
+  <si>
+    <t>CA-F6X9FP2J</t>
+  </si>
+  <si>
+    <t>CA-D3HMI2TW</t>
+  </si>
+  <si>
+    <t>CA-FYUS3P1A</t>
+  </si>
+  <si>
+    <t>CA-WYNZ34H6</t>
+  </si>
+  <si>
+    <t>CA-VX1JXGHE</t>
+  </si>
+  <si>
+    <t>CA-LQM6KOUH</t>
+  </si>
+  <si>
+    <t>CA-Z529SCHC</t>
+  </si>
+  <si>
+    <t>CA-DVJ2WQ9O</t>
+  </si>
+  <si>
+    <t>CA-2FOE2SHQ</t>
+  </si>
+  <si>
+    <t>CA-X7ZATUEO</t>
+  </si>
+  <si>
+    <t>CA-GA0RT8GP</t>
+  </si>
+  <si>
+    <t>CA-VQUSAEDS</t>
+  </si>
+  <si>
+    <t>CA-QXAGM36X</t>
+  </si>
+  <si>
+    <t>CA-I5OS3OUL</t>
   </si>
 </sst>
 </file>
@@ -570,7 +630,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
update genetics denied & cancel
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prod_tms\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43AD553-DFB6-4196-8586-C3E2DA9DB3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AB3BA7-2027-457D-A3A1-712FE1CB9F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="420">
   <si>
     <t>id</t>
   </si>
@@ -109,103 +109,1183 @@
     <t>Unity</t>
   </si>
   <si>
-    <t>Genetic Testing(Unity )</t>
-  </si>
-  <si>
     <t>DEMO GROUP 01 (Marketing Group)</t>
   </si>
   <si>
-    <t>CA-R723QKZS</t>
-  </si>
-  <si>
-    <t>CA-7NU4KR4K</t>
-  </si>
-  <si>
-    <t>CA-6GPALHPJ</t>
-  </si>
-  <si>
     <t>fail</t>
   </si>
   <si>
-    <t>CA-8KC7X7RK</t>
-  </si>
-  <si>
-    <t>CA-DNYHHAIO</t>
-  </si>
-  <si>
-    <t>CA-DFWMFRE9</t>
-  </si>
-  <si>
-    <t>CA-CU2I5L9E</t>
-  </si>
-  <si>
-    <t>CA-BNKDESZ6</t>
-  </si>
-  <si>
-    <t>CA-FR2PHPWO</t>
-  </si>
-  <si>
-    <t>CA-5EDNCJRQ</t>
-  </si>
-  <si>
-    <t>CA-NN0LBHTF</t>
-  </si>
-  <si>
-    <t>CA-2555KGWB</t>
-  </si>
-  <si>
-    <t>CA-QJPKWCFS</t>
-  </si>
-  <si>
-    <t>CA-J9JRJMAM</t>
-  </si>
-  <si>
-    <t>CA-3U12KDIS</t>
-  </si>
-  <si>
-    <t>CA-J7JBFQ38</t>
-  </si>
-  <si>
-    <t>CA-F6X9FP2J</t>
-  </si>
-  <si>
-    <t>CA-D3HMI2TW</t>
-  </si>
-  <si>
-    <t>CA-FYUS3P1A</t>
-  </si>
-  <si>
-    <t>CA-WYNZ34H6</t>
-  </si>
-  <si>
-    <t>CA-VX1JXGHE</t>
-  </si>
-  <si>
-    <t>CA-LQM6KOUH</t>
-  </si>
-  <si>
-    <t>CA-Z529SCHC</t>
-  </si>
-  <si>
-    <t>CA-DVJ2WQ9O</t>
-  </si>
-  <si>
-    <t>CA-2FOE2SHQ</t>
-  </si>
-  <si>
-    <t>CA-X7ZATUEO</t>
-  </si>
-  <si>
-    <t>CA-GA0RT8GP</t>
-  </si>
-  <si>
-    <t>CA-VQUSAEDS</t>
-  </si>
-  <si>
-    <t>CA-QXAGM36X</t>
-  </si>
-  <si>
-    <t>CA-I5OS3OUL</t>
+    <t>CA-D4HEYGZ7</t>
+  </si>
+  <si>
+    <t>Genetic Testing</t>
+  </si>
+  <si>
+    <t>CA-ZQ1M4TW7</t>
+  </si>
+  <si>
+    <t>CA-9GOHKAVF</t>
+  </si>
+  <si>
+    <t>CA-NTO8AFM5</t>
+  </si>
+  <si>
+    <t>CA-HQ9DZDQT</t>
+  </si>
+  <si>
+    <t>CA-IOXDHE03</t>
+  </si>
+  <si>
+    <t>CA-7V3OW6U2</t>
+  </si>
+  <si>
+    <t>CA-WNGTA63L</t>
+  </si>
+  <si>
+    <t>CA-6NK9GW58</t>
+  </si>
+  <si>
+    <t>CA-4UU54ED4</t>
+  </si>
+  <si>
+    <t>CA-NDUSI30D</t>
+  </si>
+  <si>
+    <t>CA-7BSNSUBH</t>
+  </si>
+  <si>
+    <t>CA-7IPIEOW0</t>
+  </si>
+  <si>
+    <t>CA-54XBXKQR</t>
+  </si>
+  <si>
+    <t>CA-9RQ6TFSW</t>
+  </si>
+  <si>
+    <t>CA-6UXCGM6Y</t>
+  </si>
+  <si>
+    <t>CA-E2K0T1Z3</t>
+  </si>
+  <si>
+    <t>CA-RGKC9ZI0</t>
+  </si>
+  <si>
+    <t>CA-THPJ9IFC</t>
+  </si>
+  <si>
+    <t>CA-9DGNDHTL</t>
+  </si>
+  <si>
+    <t>CA-S2XRKSYX</t>
+  </si>
+  <si>
+    <t>CA-TP388WG2</t>
+  </si>
+  <si>
+    <t>CA-ELCNQRKW</t>
+  </si>
+  <si>
+    <t>CA-91REBVYL</t>
+  </si>
+  <si>
+    <t>CA-ZQCSN8AQ</t>
+  </si>
+  <si>
+    <t>CA-8A7MACJL</t>
+  </si>
+  <si>
+    <t>CA-5OY4WF1U</t>
+  </si>
+  <si>
+    <t>CA-XZHELKUQ</t>
+  </si>
+  <si>
+    <t>CA-L2Q5S70J</t>
+  </si>
+  <si>
+    <t>CA-L70OXE6K</t>
+  </si>
+  <si>
+    <t>CA-7CEFMSV8</t>
+  </si>
+  <si>
+    <t>CA-V9LIBW5Y</t>
+  </si>
+  <si>
+    <t>CA-HLM9KFWQ</t>
+  </si>
+  <si>
+    <t>CA-NGWH42BL</t>
+  </si>
+  <si>
+    <t>CA-RID72VMW</t>
+  </si>
+  <si>
+    <t>CA-MP2QKUI5</t>
+  </si>
+  <si>
+    <t>CA-X8OWN8T3</t>
+  </si>
+  <si>
+    <t>CA-GPS3HRF7</t>
+  </si>
+  <si>
+    <t>CA-CEFY0U7M</t>
+  </si>
+  <si>
+    <t>CA-LYNS1HBP</t>
+  </si>
+  <si>
+    <t>CA-MIP2BJQC</t>
+  </si>
+  <si>
+    <t>CA-R544OMEQ</t>
+  </si>
+  <si>
+    <t>CA-QTNZ5F0B</t>
+  </si>
+  <si>
+    <t>CA-03R1UT0I</t>
+  </si>
+  <si>
+    <t>CA-ZNY5YS0M</t>
+  </si>
+  <si>
+    <t>CA-ZOSVWZ06</t>
+  </si>
+  <si>
+    <t>CA-WFUWKNWH</t>
+  </si>
+  <si>
+    <t>CA-4PSXIADQ</t>
+  </si>
+  <si>
+    <t>CA-IZOTH139</t>
+  </si>
+  <si>
+    <t>CA-AL2JSBPL</t>
+  </si>
+  <si>
+    <t>CA-DSW4O4QW</t>
+  </si>
+  <si>
+    <t>CA-902P4SX3</t>
+  </si>
+  <si>
+    <t>CA-HKUVEUI7</t>
+  </si>
+  <si>
+    <t>CA-D19U8XLC</t>
+  </si>
+  <si>
+    <t>CA-S1Z12LOA</t>
+  </si>
+  <si>
+    <t>CA-P4VXLRLT</t>
+  </si>
+  <si>
+    <t>CA-6ISTRHCQ</t>
+  </si>
+  <si>
+    <t>CA-P1IK8T9M</t>
+  </si>
+  <si>
+    <t>CA-ILYRHKHE</t>
+  </si>
+  <si>
+    <t>CA-C0RET7E4</t>
+  </si>
+  <si>
+    <t>CA-TZFQYQ89</t>
+  </si>
+  <si>
+    <t>CA-HX8R938Q</t>
+  </si>
+  <si>
+    <t>CA-R2GLS0M5</t>
+  </si>
+  <si>
+    <t>CA-UHUM1U6S</t>
+  </si>
+  <si>
+    <t>CA-GJ608WQ5</t>
+  </si>
+  <si>
+    <t>CA-6701DWLQ</t>
+  </si>
+  <si>
+    <t>CA-LMNZ23MI</t>
+  </si>
+  <si>
+    <t>CA-WQG9LWS0</t>
+  </si>
+  <si>
+    <t>CA-P09XW0DR</t>
+  </si>
+  <si>
+    <t>CA-VT6BKIHA</t>
+  </si>
+  <si>
+    <t>CA-E62P13A9</t>
+  </si>
+  <si>
+    <t>CA-BMO0OATW</t>
+  </si>
+  <si>
+    <t>CA-N4EDOWZD</t>
+  </si>
+  <si>
+    <t>CA-GF0DZLJL</t>
+  </si>
+  <si>
+    <t>CA-1SDB2WLB</t>
+  </si>
+  <si>
+    <t>CA-HQM8KLH4</t>
+  </si>
+  <si>
+    <t>CA-X2O51V9V</t>
+  </si>
+  <si>
+    <t>CA-DR8UCDOQ</t>
+  </si>
+  <si>
+    <t>CA-YEL16LA9</t>
+  </si>
+  <si>
+    <t>CA-B6JEU933</t>
+  </si>
+  <si>
+    <t>CA-0C7Z0I14</t>
+  </si>
+  <si>
+    <t>CA-ZEZ3V11D</t>
+  </si>
+  <si>
+    <t>CA-LY8EYQ8G</t>
+  </si>
+  <si>
+    <t>CA-N86R3F00</t>
+  </si>
+  <si>
+    <t>CA-I4034ZOC</t>
+  </si>
+  <si>
+    <t>CA-CMC2MLM9</t>
+  </si>
+  <si>
+    <t>CA-5H4GQBTD</t>
+  </si>
+  <si>
+    <t>CA-H21S3S8W</t>
+  </si>
+  <si>
+    <t>CA-HFB21QKN</t>
+  </si>
+  <si>
+    <t>CA-TV8Z33KW</t>
+  </si>
+  <si>
+    <t>CA-3XEMVRF4</t>
+  </si>
+  <si>
+    <t>CA-ACG1OM5L</t>
+  </si>
+  <si>
+    <t>CA-PQ6HV7FU</t>
+  </si>
+  <si>
+    <t>CA-XZWIEB89</t>
+  </si>
+  <si>
+    <t>CA-DVHXZQ4F</t>
+  </si>
+  <si>
+    <t>CA-QRN4RJL4</t>
+  </si>
+  <si>
+    <t>CA-9J5JTUVE</t>
+  </si>
+  <si>
+    <t>CA-7V2PVLCO</t>
+  </si>
+  <si>
+    <t>CA-5460GKM7</t>
+  </si>
+  <si>
+    <t>CA-NGJP35NS</t>
+  </si>
+  <si>
+    <t>CA-E7EJZ60U</t>
+  </si>
+  <si>
+    <t>CA-GC378ZLF</t>
+  </si>
+  <si>
+    <t>CA-O95OIGPK</t>
+  </si>
+  <si>
+    <t>CA-Z5I6SXH4</t>
+  </si>
+  <si>
+    <t>CA-VPHBXYJ3</t>
+  </si>
+  <si>
+    <t>CA-5U5EB0BQ</t>
+  </si>
+  <si>
+    <t>CA-YDJ3OD1A</t>
+  </si>
+  <si>
+    <t>CA-DG1A7G6H</t>
+  </si>
+  <si>
+    <t>CA-8BE2STPK</t>
+  </si>
+  <si>
+    <t>CA-BQ4BK9GU</t>
+  </si>
+  <si>
+    <t>CA-FQL2U40H</t>
+  </si>
+  <si>
+    <t>CA-7J8ACG3F</t>
+  </si>
+  <si>
+    <t>CA-GQF3D1P8</t>
+  </si>
+  <si>
+    <t>CA-M871EOPN</t>
+  </si>
+  <si>
+    <t>CA-66Q7G5BS</t>
+  </si>
+  <si>
+    <t>CA-KBADQSRP</t>
+  </si>
+  <si>
+    <t>CA-P6WW3XI1</t>
+  </si>
+  <si>
+    <t>CA-KITU9E1N</t>
+  </si>
+  <si>
+    <t>CA-VCAM8DLE</t>
+  </si>
+  <si>
+    <t>CA-A8W2F29M</t>
+  </si>
+  <si>
+    <t>CA-3DJDY5IS</t>
+  </si>
+  <si>
+    <t>CA-BEEDMQS6</t>
+  </si>
+  <si>
+    <t>CA-3TCF6H0P</t>
+  </si>
+  <si>
+    <t>CA-9Z0WHDGN</t>
+  </si>
+  <si>
+    <t>CA-G0WWZ2DS</t>
+  </si>
+  <si>
+    <t>CA-XA6S4Y2S</t>
+  </si>
+  <si>
+    <t>CA-9YERF5PJ</t>
+  </si>
+  <si>
+    <t>CA-AM0EJUZI</t>
+  </si>
+  <si>
+    <t>CA-YWAU9C87</t>
+  </si>
+  <si>
+    <t>CA-NECS8CIQ</t>
+  </si>
+  <si>
+    <t>CA-XQGSXR0T</t>
+  </si>
+  <si>
+    <t>CA-H1H885UI</t>
+  </si>
+  <si>
+    <t>CA-G7O3ADW9</t>
+  </si>
+  <si>
+    <t>CA-XMEE8PCM</t>
+  </si>
+  <si>
+    <t>CA-X3F9ZHGU</t>
+  </si>
+  <si>
+    <t>CA-UQCURMNX</t>
+  </si>
+  <si>
+    <t>CA-3WZG5NP2</t>
+  </si>
+  <si>
+    <t>CA-9L4ZVPMP</t>
+  </si>
+  <si>
+    <t>CA-LIGGU7XC</t>
+  </si>
+  <si>
+    <t>CA-PZ6CHX5A</t>
+  </si>
+  <si>
+    <t>CA-MYU8ZO0C</t>
+  </si>
+  <si>
+    <t>CA-UXVUKLBO</t>
+  </si>
+  <si>
+    <t>CA-KDL0L8IU</t>
+  </si>
+  <si>
+    <t>CA-8NRLF3Y6</t>
+  </si>
+  <si>
+    <t>CA-Y5XB83RK</t>
+  </si>
+  <si>
+    <t>CA-BZ7E9C8J</t>
+  </si>
+  <si>
+    <t>CA-2KYFSN0E</t>
+  </si>
+  <si>
+    <t>CA-7ESOIMLN</t>
+  </si>
+  <si>
+    <t>CA-F6AL3948</t>
+  </si>
+  <si>
+    <t>CA-84ED654Y</t>
+  </si>
+  <si>
+    <t>CA-9BABCXO6</t>
+  </si>
+  <si>
+    <t>CA-LCKIZ50Y</t>
+  </si>
+  <si>
+    <t>CA-LJ1QGC6A</t>
+  </si>
+  <si>
+    <t>CA-DRTVB7UB</t>
+  </si>
+  <si>
+    <t>CA-NNOW9933</t>
+  </si>
+  <si>
+    <t>CA-LZ3OTLIP</t>
+  </si>
+  <si>
+    <t>CA-WZGJWXUF</t>
+  </si>
+  <si>
+    <t>CA-IRKAGVGK</t>
+  </si>
+  <si>
+    <t>CA-KFJOBG7V</t>
+  </si>
+  <si>
+    <t>CA-NKDGJHDI</t>
+  </si>
+  <si>
+    <t>CA-W2EH0B6K</t>
+  </si>
+  <si>
+    <t>CA-3N86BS18</t>
+  </si>
+  <si>
+    <t>CA-CCCK54UY</t>
+  </si>
+  <si>
+    <t>CA-BIVSW8KY</t>
+  </si>
+  <si>
+    <t>CA-U1GW3YX4</t>
+  </si>
+  <si>
+    <t>CA-0TFDYZLG</t>
+  </si>
+  <si>
+    <t>CA-RDTKD2YB</t>
+  </si>
+  <si>
+    <t>CA-1IJHF70H</t>
+  </si>
+  <si>
+    <t>CA-CREIYNLO</t>
+  </si>
+  <si>
+    <t>CA-1VK5IQH8</t>
+  </si>
+  <si>
+    <t>CA-5V5D661J</t>
+  </si>
+  <si>
+    <t>CA-YCCQ9385</t>
+  </si>
+  <si>
+    <t>CA-4VGUEBQD</t>
+  </si>
+  <si>
+    <t>CA-6M1N62P5</t>
+  </si>
+  <si>
+    <t>CA-FJ38OROP</t>
+  </si>
+  <si>
+    <t>CA-YG1WEE4N</t>
+  </si>
+  <si>
+    <t>CA-VM5J15ME</t>
+  </si>
+  <si>
+    <t>CA-B8JJ6QBV</t>
+  </si>
+  <si>
+    <t>CA-X83E6FGD</t>
+  </si>
+  <si>
+    <t>CA-HOVLLT7M</t>
+  </si>
+  <si>
+    <t>CA-VFWHKHUI</t>
+  </si>
+  <si>
+    <t>CA-BG2EE117</t>
+  </si>
+  <si>
+    <t>CA-5TS3GYQR</t>
+  </si>
+  <si>
+    <t>CA-IP6A66FC</t>
+  </si>
+  <si>
+    <t>CA-D59YM8QU</t>
+  </si>
+  <si>
+    <t>CA-E3MBUQG3</t>
+  </si>
+  <si>
+    <t>CA-EBYEVGKV</t>
+  </si>
+  <si>
+    <t>CA-ICZLVZB2</t>
+  </si>
+  <si>
+    <t>CA-LUKJ6T44</t>
+  </si>
+  <si>
+    <t>CA-KOUTM71Q</t>
+  </si>
+  <si>
+    <t>CA-9YAG3AVQ</t>
+  </si>
+  <si>
+    <t>CA-HYBBATO0</t>
+  </si>
+  <si>
+    <t>CA-UWTLNY9X</t>
+  </si>
+  <si>
+    <t>CA-PGRXW33M</t>
+  </si>
+  <si>
+    <t>CA-E0FXEI8K</t>
+  </si>
+  <si>
+    <t>CA-ZNRX9DG2</t>
+  </si>
+  <si>
+    <t>CA-J3ZHKT28</t>
+  </si>
+  <si>
+    <t>CA-2LK66NKE</t>
+  </si>
+  <si>
+    <t>CA-SDU5DM5J</t>
+  </si>
+  <si>
+    <t>CA-M1KZ1HU3</t>
+  </si>
+  <si>
+    <t>CA-4YPX6Y9E</t>
+  </si>
+  <si>
+    <t>CA-E13CTSG7</t>
+  </si>
+  <si>
+    <t>CA-86UUJ4NR</t>
+  </si>
+  <si>
+    <t>CA-J0VS10SC</t>
+  </si>
+  <si>
+    <t>CA-EH9SD5ID</t>
+  </si>
+  <si>
+    <t>CA-ER2Y310S</t>
+  </si>
+  <si>
+    <t>CA-AUCACN2Y</t>
+  </si>
+  <si>
+    <t>CA-WDHUWZL7</t>
+  </si>
+  <si>
+    <t>CA-DCXK3NTD</t>
+  </si>
+  <si>
+    <t>CA-0IQSJ1LM</t>
+  </si>
+  <si>
+    <t>CA-0LZISDK6</t>
+  </si>
+  <si>
+    <t>CA-4Q6O7SSI</t>
+  </si>
+  <si>
+    <t>CA-MNLXFZXP</t>
+  </si>
+  <si>
+    <t>CA-4KQWQTIC</t>
+  </si>
+  <si>
+    <t>CA-TTHF140W</t>
+  </si>
+  <si>
+    <t>CA-MDGBZZSX</t>
+  </si>
+  <si>
+    <t>CA-N52SD1F0</t>
+  </si>
+  <si>
+    <t>CA-WIOVXAZD</t>
+  </si>
+  <si>
+    <t>CA-0P9AL9W3</t>
+  </si>
+  <si>
+    <t>CA-D9UITNFT</t>
+  </si>
+  <si>
+    <t>CA-8FR1N27F</t>
+  </si>
+  <si>
+    <t>CA-FWNQU18M</t>
+  </si>
+  <si>
+    <t>CA-RTSWOFY9</t>
+  </si>
+  <si>
+    <t>CA-12GN1GFZ</t>
+  </si>
+  <si>
+    <t>CA-I28ONBJF</t>
+  </si>
+  <si>
+    <t>CA-U6MS596Q</t>
+  </si>
+  <si>
+    <t>CA-955TOD1O</t>
+  </si>
+  <si>
+    <t>CA-8VOM6AKD</t>
+  </si>
+  <si>
+    <t>CA-HD57E44G</t>
+  </si>
+  <si>
+    <t>CA-Y7IANRHW</t>
+  </si>
+  <si>
+    <t>CA-U8OAZBMQ</t>
+  </si>
+  <si>
+    <t>CA-ABAAMN1G</t>
+  </si>
+  <si>
+    <t>CA-SIMFEEIR</t>
+  </si>
+  <si>
+    <t>CA-7Z0L6TDL</t>
+  </si>
+  <si>
+    <t>CA-YHYERRDT</t>
+  </si>
+  <si>
+    <t>CA-ELKYARJ2</t>
+  </si>
+  <si>
+    <t>CA-Q8ZVPC8F</t>
+  </si>
+  <si>
+    <t>CA-PTQ7K9UC</t>
+  </si>
+  <si>
+    <t>CA-Z92ALR64</t>
+  </si>
+  <si>
+    <t>CA-JTWIQ12Z</t>
+  </si>
+  <si>
+    <t>CA-6ZSBOPLS</t>
+  </si>
+  <si>
+    <t>CA-SNUCQVF6</t>
+  </si>
+  <si>
+    <t>CA-MGN1997F</t>
+  </si>
+  <si>
+    <t>CA-KCOODXND</t>
+  </si>
+  <si>
+    <t>CA-3ZOADZGQ</t>
+  </si>
+  <si>
+    <t>CA-BEXZ7IAP</t>
+  </si>
+  <si>
+    <t>CA-2HTSE1SU</t>
+  </si>
+  <si>
+    <t>CA-O49RZJ5T</t>
+  </si>
+  <si>
+    <t>CA-DF0YO4XD</t>
+  </si>
+  <si>
+    <t>CA-J3RGIUON</t>
+  </si>
+  <si>
+    <t>CA-6EB1K603</t>
+  </si>
+  <si>
+    <t>CA-D54ONO3E</t>
+  </si>
+  <si>
+    <t>CA-N8Q3TB5W</t>
+  </si>
+  <si>
+    <t>CA-84DKJHNM</t>
+  </si>
+  <si>
+    <t>CA-S8VOSVOV</t>
+  </si>
+  <si>
+    <t>CA-C4DC2514</t>
+  </si>
+  <si>
+    <t>CA-E4UM9RVH</t>
+  </si>
+  <si>
+    <t>CA-7GFSG670</t>
+  </si>
+  <si>
+    <t>CA-K94XI6X0</t>
+  </si>
+  <si>
+    <t>CA-ONP5G0O7</t>
+  </si>
+  <si>
+    <t>CA-R4TJFPK8</t>
+  </si>
+  <si>
+    <t>CA-B1BUBVXN</t>
+  </si>
+  <si>
+    <t>CA-IOB63G36</t>
+  </si>
+  <si>
+    <t>CA-9RL5D4ST</t>
+  </si>
+  <si>
+    <t>CA-EIBZWKV1</t>
+  </si>
+  <si>
+    <t>CA-NFEYT1FY</t>
+  </si>
+  <si>
+    <t>CA-YMZS2UG5</t>
+  </si>
+  <si>
+    <t>CA-PHYOMYX4</t>
+  </si>
+  <si>
+    <t>CA-PRLX3ZGM</t>
+  </si>
+  <si>
+    <t>CA-Z0C2E4UR</t>
+  </si>
+  <si>
+    <t>CA-T3E42N00</t>
+  </si>
+  <si>
+    <t>CA-TJYLR4DR</t>
+  </si>
+  <si>
+    <t>CA-Z16U944G</t>
+  </si>
+  <si>
+    <t>CA-TD04N3G1</t>
+  </si>
+  <si>
+    <t>CA-4GJZ8K5Z</t>
+  </si>
+  <si>
+    <t>CA-EPR7H5YY</t>
+  </si>
+  <si>
+    <t>CA-R7Q2M3EE</t>
+  </si>
+  <si>
+    <t>CA-2JBQMKQM</t>
+  </si>
+  <si>
+    <t>CA-5K3SVHAN</t>
+  </si>
+  <si>
+    <t>CA-4CA1JUYH</t>
+  </si>
+  <si>
+    <t>CA-SWOZR9GS</t>
+  </si>
+  <si>
+    <t>CA-SR7QZBUY</t>
+  </si>
+  <si>
+    <t>CA-W25ZOPKQ</t>
+  </si>
+  <si>
+    <t>CA-ZP232NZK</t>
+  </si>
+  <si>
+    <t>CA-2EF6G8L3</t>
+  </si>
+  <si>
+    <t>CA-8BQUGBEM</t>
+  </si>
+  <si>
+    <t>CA-499EAI35</t>
+  </si>
+  <si>
+    <t>CA-PP6925HK</t>
+  </si>
+  <si>
+    <t>CA-QQXJE1C7</t>
+  </si>
+  <si>
+    <t>CA-IUPWSQ7K</t>
+  </si>
+  <si>
+    <t>CA-819IBA6B</t>
+  </si>
+  <si>
+    <t>CA-VA8K3TSR</t>
+  </si>
+  <si>
+    <t>CA-9K75HYVI</t>
+  </si>
+  <si>
+    <t>CA-KR9TP8KD</t>
+  </si>
+  <si>
+    <t>CA-50GPU7ES</t>
+  </si>
+  <si>
+    <t>CA-LGVDBJ5Z</t>
+  </si>
+  <si>
+    <t>CA-276GWH0T</t>
+  </si>
+  <si>
+    <t>CA-0D0T5EKW</t>
+  </si>
+  <si>
+    <t>CA-AL3DRX5U</t>
+  </si>
+  <si>
+    <t>CA-7MV6Z4HC</t>
+  </si>
+  <si>
+    <t>CA-1M46YZ24</t>
+  </si>
+  <si>
+    <t>CA-UVMR0CBQ</t>
+  </si>
+  <si>
+    <t>CA-SPP7CQVH</t>
+  </si>
+  <si>
+    <t>CA-LBY59FTY</t>
+  </si>
+  <si>
+    <t>CA-Y27T1CJK</t>
+  </si>
+  <si>
+    <t>CA-JVW3NICS</t>
+  </si>
+  <si>
+    <t>CA-LKFODO6G</t>
+  </si>
+  <si>
+    <t>CA-00E4678Q</t>
+  </si>
+  <si>
+    <t>CA-E8YOXDWQ</t>
+  </si>
+  <si>
+    <t>CA-NNRLO0MA</t>
+  </si>
+  <si>
+    <t>CA-TS0WUWBN</t>
+  </si>
+  <si>
+    <t>CA-5O08XYQP</t>
+  </si>
+  <si>
+    <t>CA-ECIFIMUO</t>
+  </si>
+  <si>
+    <t>CA-R4XVK85S</t>
+  </si>
+  <si>
+    <t>CA-5O6V9RYE</t>
+  </si>
+  <si>
+    <t>CA-C17UXIP4</t>
+  </si>
+  <si>
+    <t>CA-S3Q5C2S6</t>
+  </si>
+  <si>
+    <t>CA-0I7L7CQO</t>
+  </si>
+  <si>
+    <t>CA-50AMRG0H</t>
+  </si>
+  <si>
+    <t>CA-NSZFSLUU</t>
+  </si>
+  <si>
+    <t>CA-9WZGDRN6</t>
+  </si>
+  <si>
+    <t>CA-8H9FKMNQ</t>
+  </si>
+  <si>
+    <t>CA-IMCB0W81</t>
+  </si>
+  <si>
+    <t>CA-YGONFHID</t>
+  </si>
+  <si>
+    <t>CA-WZE0PR24</t>
+  </si>
+  <si>
+    <t>CA-J9OZE1MF</t>
+  </si>
+  <si>
+    <t>CA-TNGU29P8</t>
+  </si>
+  <si>
+    <t>CA-I6R0ZTNZ</t>
+  </si>
+  <si>
+    <t>CA-YJZT4UZR</t>
+  </si>
+  <si>
+    <t>CA-9S1J49M4</t>
+  </si>
+  <si>
+    <t>CA-KX4BUWC3</t>
+  </si>
+  <si>
+    <t>CA-H1TF9GY3</t>
+  </si>
+  <si>
+    <t>CA-YGJI26G5</t>
+  </si>
+  <si>
+    <t>CA-U2P9K12R</t>
+  </si>
+  <si>
+    <t>CA-X6MMJU2Z</t>
+  </si>
+  <si>
+    <t>CA-QFSPWISC</t>
+  </si>
+  <si>
+    <t>CA-YWDME48U</t>
+  </si>
+  <si>
+    <t>CA-V22EIF4A</t>
+  </si>
+  <si>
+    <t>CA-R7G6M7E2</t>
+  </si>
+  <si>
+    <t>CA-NYKGTL2Y</t>
+  </si>
+  <si>
+    <t>CA-UPM0RCWV</t>
+  </si>
+  <si>
+    <t>CA-OOZ5CNWQ</t>
+  </si>
+  <si>
+    <t>CA-AIX9TFC3</t>
+  </si>
+  <si>
+    <t>CA-5T5CR9S6</t>
+  </si>
+  <si>
+    <t>CA-X0ZVJ8GI</t>
+  </si>
+  <si>
+    <t>CA-ER9MQ6IX</t>
+  </si>
+  <si>
+    <t>CA-Z021F2UM</t>
+  </si>
+  <si>
+    <t>CA-UXQ2B1TH</t>
+  </si>
+  <si>
+    <t>CA-NKO22OM3</t>
+  </si>
+  <si>
+    <t>CA-QIJXR80V</t>
+  </si>
+  <si>
+    <t>CA-TFA1V0G7</t>
+  </si>
+  <si>
+    <t>CA-YHM2BV7J</t>
+  </si>
+  <si>
+    <t>CA-IJ3K8YQ4</t>
+  </si>
+  <si>
+    <t>CA-OCUQ3FTV</t>
+  </si>
+  <si>
+    <t>CA-YW5ET0T7</t>
+  </si>
+  <si>
+    <t>CA-WV2NCRQ6</t>
+  </si>
+  <si>
+    <t>CA-2T09YFGE</t>
+  </si>
+  <si>
+    <t>CA-VKSUW1A8</t>
+  </si>
+  <si>
+    <t>CA-9RZVMLQW</t>
+  </si>
+  <si>
+    <t>CA-RQJCAUB8</t>
+  </si>
+  <si>
+    <t>CA-ELSJKY6V</t>
+  </si>
+  <si>
+    <t>CA-R564AIWB</t>
+  </si>
+  <si>
+    <t>CA-PZ5ZL0R0</t>
+  </si>
+  <si>
+    <t>CA-QQNR1IWV</t>
+  </si>
+  <si>
+    <t>CA-0VI0XFDC</t>
+  </si>
+  <si>
+    <t>CA-JZ3AY120</t>
+  </si>
+  <si>
+    <t>CA-MB8TUVD2</t>
+  </si>
+  <si>
+    <t>CA-YU8DFHRY</t>
+  </si>
+  <si>
+    <t>CA-MADSN28E</t>
+  </si>
+  <si>
+    <t>CA-RDK6Q4EO</t>
+  </si>
+  <si>
+    <t>CA-A7MHFJGM</t>
+  </si>
+  <si>
+    <t>CA-5FMOXVFH</t>
+  </si>
+  <si>
+    <t>CA-AIZ0C8IO</t>
+  </si>
+  <si>
+    <t>CA-Z5BWCN7B</t>
+  </si>
+  <si>
+    <t>CA-56JYGKP7</t>
+  </si>
+  <si>
+    <t>CA-FQPWZQKJ</t>
+  </si>
+  <si>
+    <t>CA-J9HAIZU3</t>
+  </si>
+  <si>
+    <t>CA-JZJRONSS</t>
+  </si>
+  <si>
+    <t>CA-UKNM47HS</t>
+  </si>
+  <si>
+    <t>CA-8RPYC55F</t>
+  </si>
+  <si>
+    <t>CA-M2SR567Y</t>
+  </si>
+  <si>
+    <t>CA-EKJC6X80</t>
+  </si>
+  <si>
+    <t>CA-W8DP1BSF</t>
+  </si>
+  <si>
+    <t>CA-58OPO738</t>
+  </si>
+  <si>
+    <t>CA-P1YG6LPS</t>
+  </si>
+  <si>
+    <t>CA-MB8O86NA</t>
+  </si>
+  <si>
+    <t>CA-4ZESB0WP</t>
+  </si>
+  <si>
+    <t>CA-WKJOROAC</t>
+  </si>
+  <si>
+    <t>CA-IPMMJC20</t>
+  </si>
+  <si>
+    <t>CA-39IONHI7</t>
   </si>
 </sst>
 </file>
@@ -576,7 +1656,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,16 +1710,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>419</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -727,7 +1807,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update core tms 1&2
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>id</t>
   </si>
@@ -134,6 +134,66 @@
   </si>
   <si>
     <t>CA-5XAUJ6J3</t>
+  </si>
+  <si>
+    <t>CA-8VQU5JON</t>
+  </si>
+  <si>
+    <t>CA-HV0Q2QO6</t>
+  </si>
+  <si>
+    <t>CA-OGGR4TFW</t>
+  </si>
+  <si>
+    <t>CA-O3DT2O4N</t>
+  </si>
+  <si>
+    <t>CA-M4Y5LD7C</t>
+  </si>
+  <si>
+    <t>CA-BVNNTX6W</t>
+  </si>
+  <si>
+    <t>CA-ERZ65MUJ</t>
+  </si>
+  <si>
+    <t>CA-6FOLWCYU</t>
+  </si>
+  <si>
+    <t>CA-B5VRQA3O</t>
+  </si>
+  <si>
+    <t>CA-09DBNCBD</t>
+  </si>
+  <si>
+    <t>CA-WROJLHRU</t>
+  </si>
+  <si>
+    <t>CA-9BTNQ9P5</t>
+  </si>
+  <si>
+    <t>CA-PBKTFB4J</t>
+  </si>
+  <si>
+    <t>CA-17FVX4JR</t>
+  </si>
+  <si>
+    <t>CA-PE3IBFTF</t>
+  </si>
+  <si>
+    <t>CA-HQ5DMDIF</t>
+  </si>
+  <si>
+    <t>CA-HGTFBRXD</t>
+  </si>
+  <si>
+    <t>CA-UKCN552Z</t>
+  </si>
+  <si>
+    <t>CA-8KSNSTAD</t>
+  </si>
+  <si>
+    <t>CA-TVP8RWH8</t>
   </si>
 </sst>
 </file>
@@ -558,7 +618,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
udpate core tms & telehealth
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="772">
   <si>
     <t>id</t>
   </si>
@@ -2328,6 +2328,21 @@
   </si>
   <si>
     <t>CA-33W83HN3</t>
+  </si>
+  <si>
+    <t>CA-AXZK3VWQ</t>
+  </si>
+  <si>
+    <t>CA-TWDDTIUP</t>
+  </si>
+  <si>
+    <t>CA-SPEH99OQ</t>
+  </si>
+  <si>
+    <t>CA-IIZ1PUO6</t>
+  </si>
+  <si>
+    <t>CA-ZP7YWM37</t>
   </si>
 </sst>
 </file>
@@ -2762,7 +2777,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>766</v>
+        <v>771</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
update xpath dom for ele
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="847">
   <si>
     <t>id</t>
   </si>
@@ -2343,6 +2343,231 @@
   </si>
   <si>
     <t>CA-ZP7YWM37</t>
+  </si>
+  <si>
+    <t>CA-76NOU7JS</t>
+  </si>
+  <si>
+    <t>CA-ENJ0BZX3</t>
+  </si>
+  <si>
+    <t>CA-8MNPS98B</t>
+  </si>
+  <si>
+    <t>CA-MKOT1XNS</t>
+  </si>
+  <si>
+    <t>CA-JELFXYZK</t>
+  </si>
+  <si>
+    <t>CA-6RQI90HP</t>
+  </si>
+  <si>
+    <t>CA-N6L0LYTQ</t>
+  </si>
+  <si>
+    <t>CA-GYFB2E78</t>
+  </si>
+  <si>
+    <t>CA-2ZGBSRBW</t>
+  </si>
+  <si>
+    <t>CA-8NZP6UGF</t>
+  </si>
+  <si>
+    <t>CA-1TDCVNTE</t>
+  </si>
+  <si>
+    <t>CA-3RW1H4V2</t>
+  </si>
+  <si>
+    <t>CA-DEILLOGC</t>
+  </si>
+  <si>
+    <t>CA-F2F3UKU4</t>
+  </si>
+  <si>
+    <t>CA-OZ92X7H8</t>
+  </si>
+  <si>
+    <t>CA-36GKRSXA</t>
+  </si>
+  <si>
+    <t>CA-MCWO5ZAT</t>
+  </si>
+  <si>
+    <t>CA-S4778J81</t>
+  </si>
+  <si>
+    <t>CA-WS3FATPZ</t>
+  </si>
+  <si>
+    <t>CA-KBQWIRM9</t>
+  </si>
+  <si>
+    <t>CA-R3LW9WR0</t>
+  </si>
+  <si>
+    <t>CA-BGSHBYPH</t>
+  </si>
+  <si>
+    <t>CA-A4S4N6JF</t>
+  </si>
+  <si>
+    <t>CA-KQC04MSF</t>
+  </si>
+  <si>
+    <t>CA-6RCXO4J6</t>
+  </si>
+  <si>
+    <t>CA-R59P5OHY</t>
+  </si>
+  <si>
+    <t>CA-1YGYPERH</t>
+  </si>
+  <si>
+    <t>CA-HACNOFUS</t>
+  </si>
+  <si>
+    <t>CA-UKIOGWQ4</t>
+  </si>
+  <si>
+    <t>CA-2TI2EO7N</t>
+  </si>
+  <si>
+    <t>CA-447HIZF8</t>
+  </si>
+  <si>
+    <t>CA-MG3V1DGN</t>
+  </si>
+  <si>
+    <t>CA-T93CKQZL</t>
+  </si>
+  <si>
+    <t>CA-IY78NF52</t>
+  </si>
+  <si>
+    <t>CA-PX9QYINR</t>
+  </si>
+  <si>
+    <t>CA-98JUNOLC</t>
+  </si>
+  <si>
+    <t>CA-GT0N0NZX</t>
+  </si>
+  <si>
+    <t>CA-JLGTWY6P</t>
+  </si>
+  <si>
+    <t>CA-WN7TDWFD</t>
+  </si>
+  <si>
+    <t>CA-N16K116A</t>
+  </si>
+  <si>
+    <t>CA-0PS1CIRR</t>
+  </si>
+  <si>
+    <t>CA-4FX8J2U8</t>
+  </si>
+  <si>
+    <t>CA-3AXB2B3W</t>
+  </si>
+  <si>
+    <t>CA-PAJ61WJN</t>
+  </si>
+  <si>
+    <t>CA-QQX487R5</t>
+  </si>
+  <si>
+    <t>CA-T7BDL43Q</t>
+  </si>
+  <si>
+    <t>CA-9DUOON00</t>
+  </si>
+  <si>
+    <t>CA-YEDZQFW9</t>
+  </si>
+  <si>
+    <t>CA-HZLCC2SF</t>
+  </si>
+  <si>
+    <t>CA-YI3A6PT4</t>
+  </si>
+  <si>
+    <t>CA-LUYW2PMT</t>
+  </si>
+  <si>
+    <t>CA-OJCSM0JK</t>
+  </si>
+  <si>
+    <t>CA-NS0PXRKW</t>
+  </si>
+  <si>
+    <t>CA-RCKX8411</t>
+  </si>
+  <si>
+    <t>CA-CVKBUL7D</t>
+  </si>
+  <si>
+    <t>CA-QQV3CVJX</t>
+  </si>
+  <si>
+    <t>CA-2IZHNT89</t>
+  </si>
+  <si>
+    <t>CA-7VX4847H</t>
+  </si>
+  <si>
+    <t>CA-X8O1FKQN</t>
+  </si>
+  <si>
+    <t>CA-DX72LRS5</t>
+  </si>
+  <si>
+    <t>CA-2W45CXT2</t>
+  </si>
+  <si>
+    <t>CA-ICGZW2GY</t>
+  </si>
+  <si>
+    <t>CA-1BGAK2QJ</t>
+  </si>
+  <si>
+    <t>CA-BQAX9QP3</t>
+  </si>
+  <si>
+    <t>CA-ONS9HW9N</t>
+  </si>
+  <si>
+    <t>CA-UI82UPKY</t>
+  </si>
+  <si>
+    <t>CA-94PQ5YOP</t>
+  </si>
+  <si>
+    <t>CA-OHBW3GFK</t>
+  </si>
+  <si>
+    <t>CA-55AH6UPI</t>
+  </si>
+  <si>
+    <t>CA-YYUBAAV2</t>
+  </si>
+  <si>
+    <t>CA-A4S8IUGQ</t>
+  </si>
+  <si>
+    <t>CA-QRW3NIY4</t>
+  </si>
+  <si>
+    <t>CA-2HN4J9FH</t>
+  </si>
+  <si>
+    <t>CA-S84ONCRG</t>
+  </si>
+  <si>
+    <t>CA-G1G7P45L</t>
   </si>
 </sst>
 </file>
@@ -2777,7 +3002,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>771</v>
+        <v>846</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
update core 16 May
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="850">
   <si>
     <t>id</t>
   </si>
@@ -2568,6 +2568,15 @@
   </si>
   <si>
     <t>CA-G1G7P45L</t>
+  </si>
+  <si>
+    <t>CA-D8FA9900</t>
+  </si>
+  <si>
+    <t>CA-PYNK4931</t>
+  </si>
+  <si>
+    <t>CA-LQD7KEE1</t>
   </si>
 </sst>
 </file>
@@ -3002,7 +3011,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
change cgx to pgx
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prod_tms\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0DC1AB-3E54-4EF9-ACE6-E38FB87CA8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CAF3B7-4DD6-492A-8740-D7BE804BD1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35100" yWindow="2190" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="762">
   <si>
     <t>id</t>
   </si>
@@ -95,9 +95,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>CGX</t>
-  </si>
-  <si>
     <t>cgx</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>genetics</t>
   </si>
   <si>
-    <t>CGX - Biogroup</t>
-  </si>
-  <si>
     <t>created_at</t>
   </si>
   <si>
@@ -2300,310 +2294,25 @@
     <t>6TR7FG7RT37</t>
   </si>
   <si>
-    <t>CA-6WRQ180A</t>
-  </si>
-  <si>
-    <t>CA-GUKP9OZ0</t>
-  </si>
-  <si>
-    <t>CA-FLJVW5OO</t>
-  </si>
-  <si>
-    <t>CA-U3MTUV8F</t>
-  </si>
-  <si>
-    <t>CA-KI5OAFQ5</t>
-  </si>
-  <si>
-    <t>CA-KOJW8KN7</t>
-  </si>
-  <si>
-    <t>CA-PM20TJHI</t>
-  </si>
-  <si>
-    <t>CA-HTFDROES</t>
-  </si>
-  <si>
-    <t>CA-OGI6HC7D</t>
-  </si>
-  <si>
-    <t>CA-33W83HN3</t>
-  </si>
-  <si>
-    <t>CA-AXZK3VWQ</t>
-  </si>
-  <si>
-    <t>CA-TWDDTIUP</t>
-  </si>
-  <si>
-    <t>CA-SPEH99OQ</t>
-  </si>
-  <si>
-    <t>CA-IIZ1PUO6</t>
-  </si>
-  <si>
-    <t>CA-ZP7YWM37</t>
-  </si>
-  <si>
-    <t>CA-76NOU7JS</t>
-  </si>
-  <si>
-    <t>CA-ENJ0BZX3</t>
-  </si>
-  <si>
-    <t>CA-8MNPS98B</t>
-  </si>
-  <si>
-    <t>CA-MKOT1XNS</t>
-  </si>
-  <si>
-    <t>CA-JELFXYZK</t>
-  </si>
-  <si>
-    <t>CA-6RQI90HP</t>
-  </si>
-  <si>
-    <t>CA-N6L0LYTQ</t>
-  </si>
-  <si>
-    <t>CA-GYFB2E78</t>
-  </si>
-  <si>
-    <t>CA-2ZGBSRBW</t>
-  </si>
-  <si>
-    <t>CA-8NZP6UGF</t>
-  </si>
-  <si>
-    <t>CA-1TDCVNTE</t>
-  </si>
-  <si>
-    <t>CA-3RW1H4V2</t>
-  </si>
-  <si>
-    <t>CA-DEILLOGC</t>
-  </si>
-  <si>
-    <t>CA-F2F3UKU4</t>
-  </si>
-  <si>
-    <t>CA-OZ92X7H8</t>
-  </si>
-  <si>
-    <t>CA-36GKRSXA</t>
-  </si>
-  <si>
-    <t>CA-MCWO5ZAT</t>
-  </si>
-  <si>
-    <t>CA-S4778J81</t>
-  </si>
-  <si>
-    <t>CA-WS3FATPZ</t>
-  </si>
-  <si>
-    <t>CA-KBQWIRM9</t>
-  </si>
-  <si>
-    <t>CA-R3LW9WR0</t>
-  </si>
-  <si>
-    <t>CA-BGSHBYPH</t>
-  </si>
-  <si>
-    <t>CA-A4S4N6JF</t>
-  </si>
-  <si>
-    <t>CA-KQC04MSF</t>
-  </si>
-  <si>
-    <t>CA-6RCXO4J6</t>
-  </si>
-  <si>
-    <t>CA-R59P5OHY</t>
-  </si>
-  <si>
-    <t>CA-1YGYPERH</t>
-  </si>
-  <si>
-    <t>CA-HACNOFUS</t>
-  </si>
-  <si>
-    <t>CA-UKIOGWQ4</t>
-  </si>
-  <si>
-    <t>CA-2TI2EO7N</t>
-  </si>
-  <si>
-    <t>CA-447HIZF8</t>
-  </si>
-  <si>
-    <t>CA-MG3V1DGN</t>
-  </si>
-  <si>
-    <t>CA-T93CKQZL</t>
-  </si>
-  <si>
-    <t>CA-IY78NF52</t>
-  </si>
-  <si>
-    <t>CA-PX9QYINR</t>
-  </si>
-  <si>
-    <t>CA-98JUNOLC</t>
-  </si>
-  <si>
-    <t>CA-GT0N0NZX</t>
-  </si>
-  <si>
-    <t>CA-JLGTWY6P</t>
-  </si>
-  <si>
-    <t>CA-WN7TDWFD</t>
-  </si>
-  <si>
-    <t>CA-N16K116A</t>
-  </si>
-  <si>
-    <t>CA-0PS1CIRR</t>
-  </si>
-  <si>
-    <t>CA-4FX8J2U8</t>
-  </si>
-  <si>
-    <t>CA-3AXB2B3W</t>
-  </si>
-  <si>
-    <t>CA-PAJ61WJN</t>
-  </si>
-  <si>
-    <t>CA-QQX487R5</t>
-  </si>
-  <si>
-    <t>CA-T7BDL43Q</t>
-  </si>
-  <si>
-    <t>CA-9DUOON00</t>
-  </si>
-  <si>
-    <t>CA-YEDZQFW9</t>
-  </si>
-  <si>
-    <t>CA-HZLCC2SF</t>
-  </si>
-  <si>
-    <t>CA-YI3A6PT4</t>
-  </si>
-  <si>
-    <t>CA-LUYW2PMT</t>
-  </si>
-  <si>
-    <t>CA-OJCSM0JK</t>
-  </si>
-  <si>
-    <t>CA-NS0PXRKW</t>
-  </si>
-  <si>
-    <t>CA-RCKX8411</t>
-  </si>
-  <si>
-    <t>CA-CVKBUL7D</t>
-  </si>
-  <si>
-    <t>CA-QQV3CVJX</t>
-  </si>
-  <si>
-    <t>CA-2IZHNT89</t>
-  </si>
-  <si>
-    <t>CA-7VX4847H</t>
-  </si>
-  <si>
-    <t>CA-X8O1FKQN</t>
-  </si>
-  <si>
-    <t>CA-DX72LRS5</t>
-  </si>
-  <si>
-    <t>CA-2W45CXT2</t>
-  </si>
-  <si>
-    <t>CA-ICGZW2GY</t>
-  </si>
-  <si>
-    <t>CA-1BGAK2QJ</t>
-  </si>
-  <si>
-    <t>CA-BQAX9QP3</t>
-  </si>
-  <si>
-    <t>CA-ONS9HW9N</t>
-  </si>
-  <si>
-    <t>CA-UI82UPKY</t>
-  </si>
-  <si>
-    <t>CA-94PQ5YOP</t>
-  </si>
-  <si>
-    <t>CA-OHBW3GFK</t>
-  </si>
-  <si>
-    <t>CA-55AH6UPI</t>
-  </si>
-  <si>
-    <t>CA-YYUBAAV2</t>
-  </si>
-  <si>
-    <t>CA-A4S8IUGQ</t>
-  </si>
-  <si>
-    <t>CA-QRW3NIY4</t>
-  </si>
-  <si>
-    <t>CA-2HN4J9FH</t>
-  </si>
-  <si>
-    <t>CA-S84ONCRG</t>
-  </si>
-  <si>
-    <t>CA-G1G7P45L</t>
-  </si>
-  <si>
-    <t>CA-D8FA9900</t>
-  </si>
-  <si>
-    <t>CA-PYNK4931</t>
-  </si>
-  <si>
-    <t>CA-LQD7KEE1</t>
-  </si>
-  <si>
-    <t>CA-TGPVHYLW</t>
-  </si>
-  <si>
-    <t>CA-QPTDDNUK</t>
-  </si>
-  <si>
-    <t>CA-4CWTA9DA</t>
-  </si>
-  <si>
-    <t>CA-G1ZQC5ZM</t>
-  </si>
-  <si>
-    <t>CA-YM7I16W6</t>
-  </si>
-  <si>
-    <t>CA-IF09XOV7</t>
-  </si>
-  <si>
-    <t>CA-YUF3KBII</t>
-  </si>
-  <si>
-    <t>CA-PCEY0WA5</t>
-  </si>
-  <si>
-    <t>CA-VA1OIJLO</t>
+    <t>PGX - GeneTX Apr 2024</t>
+  </si>
+  <si>
+    <t>PGX</t>
+  </si>
+  <si>
+    <t>CA-8HQI316G</t>
+  </si>
+  <si>
+    <t>CA-N6QYX7V2</t>
+  </si>
+  <si>
+    <t>CA-99KQDLJN</t>
+  </si>
+  <si>
+    <t>CA-FUJ1K46M</t>
+  </si>
+  <si>
+    <t>CA-8GG7VCCH</t>
   </si>
 </sst>
 </file>
@@ -2613,7 +2322,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2637,6 +2346,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2687,7 +2402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2701,6 +2416,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -2984,7 +2700,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3038,34 +2754,34 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>858</v>
+        <v>761</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>28</v>
+        <v>756</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>755</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="K2">
         <v>10010</v>
@@ -3135,7 +2851,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25.5">
@@ -3175,3409 +2891,3409 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>461</v>
+      </c>
+      <c r="H1" t="s">
         <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>463</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E2" s="7">
         <v>19218</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E3" s="7">
         <v>16435</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B4" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E4" s="7">
         <v>13863</v>
       </c>
       <c r="F4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G4" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" s="7">
         <v>20294</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E6" s="7">
         <v>14997</v>
       </c>
       <c r="F6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B7" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E7" s="7">
         <v>16111</v>
       </c>
       <c r="F7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G7" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E8" s="7">
         <v>30897</v>
       </c>
       <c r="F8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G8" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B9" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E9" s="7">
         <v>18449</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B10" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E10" s="7">
         <v>20068</v>
       </c>
       <c r="F10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G10" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B11" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E11" s="7">
         <v>17340</v>
       </c>
       <c r="F11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G11" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E12" s="7">
         <v>12390</v>
       </c>
       <c r="F12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B13" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E13" s="7">
         <v>10926</v>
       </c>
       <c r="F13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B14" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E14" s="7">
         <v>16514</v>
       </c>
       <c r="F14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G14" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B15" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E15" s="7">
         <v>18486</v>
       </c>
       <c r="F15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G15" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B16" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E16" s="7">
         <v>12812</v>
       </c>
       <c r="F16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G16" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B17" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E17" s="7">
         <v>18665</v>
       </c>
       <c r="F17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G17" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B18" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E18" s="7">
         <v>17120</v>
       </c>
       <c r="F18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G18" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B19" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E19" s="7">
         <v>15756</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G19" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B20" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C20" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D20" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E20" s="7">
         <v>17436</v>
       </c>
       <c r="F20" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G20" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B21" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E21" s="7">
         <v>12936</v>
       </c>
       <c r="F21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G21" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B22" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E22" s="7">
         <v>25882</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G22" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B23" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E23" s="7">
         <v>17460</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E24" s="7">
         <v>18099</v>
       </c>
       <c r="F24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G24" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B25" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E25" s="7">
         <v>12317</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B26" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E26" s="7">
         <v>14306</v>
       </c>
       <c r="F26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G26" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B27" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E27" s="7">
         <v>16361</v>
       </c>
       <c r="F27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G27" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B28" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D28" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E28" s="7">
         <v>27895</v>
       </c>
       <c r="F28" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G28" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B29" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E29" s="7">
         <v>27792</v>
       </c>
       <c r="F29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G29" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B30" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E30" s="7">
         <v>13002</v>
       </c>
       <c r="F30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G30" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B31" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E31" s="7">
         <v>20171</v>
       </c>
       <c r="F31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G31" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B32" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E32" s="7">
         <v>14533</v>
       </c>
       <c r="F32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G32" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B33" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E33" s="7">
         <v>29012</v>
       </c>
       <c r="F33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G33" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B34" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E34" s="7">
         <v>18995</v>
       </c>
       <c r="F34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G34" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B35" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E35" s="7">
         <v>21075</v>
       </c>
       <c r="F35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G35" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B36" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D36" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E36" s="7">
         <v>14832</v>
       </c>
       <c r="F36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G36" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B37" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E37" s="7">
         <v>22936</v>
       </c>
       <c r="F37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B38" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E38" s="7">
         <v>19776</v>
       </c>
       <c r="F38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G38" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B39" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E39" s="7">
         <v>17799</v>
       </c>
       <c r="F39" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G39" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B40" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D40" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E40" s="7">
         <v>14832</v>
       </c>
       <c r="F40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G40" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B41" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C41" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D41" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E41" s="7">
         <v>13251</v>
       </c>
       <c r="F41" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G41" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B42" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E42" s="7">
         <v>19158</v>
       </c>
       <c r="F42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G42" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B43" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E43" s="7">
         <v>18098</v>
       </c>
       <c r="F43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G43" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B44" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D44" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E44" s="7">
         <v>18080</v>
       </c>
       <c r="F44" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G44" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B45" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C45" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E45" s="7">
         <v>18098</v>
       </c>
       <c r="F45" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G45" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B46" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C46" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D46" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E46" s="7">
         <v>17292</v>
       </c>
       <c r="F46" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G46" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B47" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C47" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D47" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E47" s="7">
         <v>14405</v>
       </c>
       <c r="F47" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G47" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B48" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C48" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D48" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E48" s="7">
         <v>21927</v>
       </c>
       <c r="F48" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G48" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B49" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D49" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E49" s="7">
         <v>18995</v>
       </c>
       <c r="F49" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G49" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B50" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C50" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D50" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E50" s="7">
         <v>15935</v>
       </c>
       <c r="F50" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G50" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B51" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D51" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E51" s="7">
         <v>15815</v>
       </c>
       <c r="F51" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G51" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B52" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C52" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D52" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E52" s="7">
         <v>21383</v>
       </c>
       <c r="F52" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G52" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B53" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C53" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E53" s="7">
         <v>17611</v>
       </c>
       <c r="F53" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G53" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B54" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C54" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D54" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E54" s="7">
         <v>13752</v>
       </c>
       <c r="F54" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G54" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B55" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C55" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D55" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E55" s="7">
         <v>18682</v>
       </c>
       <c r="F55" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G55" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B56" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C56" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D56" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E56" s="7">
         <v>17224</v>
       </c>
       <c r="F56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G56" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B57" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C57" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D57" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E57" s="7">
         <v>16425</v>
       </c>
       <c r="F57" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G57" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B58" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C58" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D58" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E58" s="7">
         <v>17340</v>
       </c>
       <c r="F58" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G58" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B59" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C59" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D59" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E59" s="7">
         <v>18030</v>
       </c>
       <c r="F59" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G59" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B60" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C60" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D60" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E60" s="7">
         <v>17825</v>
       </c>
       <c r="F60" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G60" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B61" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C61" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D61" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E61" s="7">
         <v>19013</v>
       </c>
       <c r="F61" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G61" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B62" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C62" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D62" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E62" s="7">
         <v>18053</v>
       </c>
       <c r="F62" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G62" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B63" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C63" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E63" s="7">
         <v>13017</v>
       </c>
       <c r="F63" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G63" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B64" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C64" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D64" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E64" s="7">
         <v>21569</v>
       </c>
       <c r="F64" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G64" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B65" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C65" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D65" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E65" s="7">
         <v>15727</v>
       </c>
       <c r="F65" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G65" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B66" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C66" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D66" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E66" s="7">
         <v>18765</v>
       </c>
       <c r="F66" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G66" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B67" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C67" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D67" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E67" s="7">
         <v>13963</v>
       </c>
       <c r="F67" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G67" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B68" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C68" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D68" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E68" s="7">
         <v>18400</v>
       </c>
       <c r="F68" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G68" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B69" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C69" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D69" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E69" s="7">
         <v>14443</v>
       </c>
       <c r="F69" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G69" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B70" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C70" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D70" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E70" s="7">
         <v>19151</v>
       </c>
       <c r="F70" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G70" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B71" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C71" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D71" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E71" s="7">
         <v>18686</v>
       </c>
       <c r="F71" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G71" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B72" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C72" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E72" s="7">
         <v>17224</v>
       </c>
       <c r="F72" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G72" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B73" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C73" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D73" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E73" s="7">
         <v>15616</v>
       </c>
       <c r="F73" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G73" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B74" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C74" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D74" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E74" s="7">
         <v>19458</v>
       </c>
       <c r="F74" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G74" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B75" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C75" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D75" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E75" s="7">
         <v>13889</v>
       </c>
       <c r="F75" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G75" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B76" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C76" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D76" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E76" s="7">
         <v>16191</v>
       </c>
       <c r="F76" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G76" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B77" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C77" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D77" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E77" s="7">
         <v>20876</v>
       </c>
       <c r="F77" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G77" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B78" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D78" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E78" s="7">
         <v>18067</v>
       </c>
       <c r="F78" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G78" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B79" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C79" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D79" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E79" s="7">
         <v>13271</v>
       </c>
       <c r="F79" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G79" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B80" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C80" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D80" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E80" s="7">
         <v>17224</v>
       </c>
       <c r="F80" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G80" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B81" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C81" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D81" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E81" s="7">
         <v>21375</v>
       </c>
       <c r="F81" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G81" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B82" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C82" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D82" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E82" s="7">
         <v>18010</v>
       </c>
       <c r="F82" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G82" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B83" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C83" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D83" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E83" s="7">
         <v>14830</v>
       </c>
       <c r="F83" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G83" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B84" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C84" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D84" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E84" s="7">
         <v>19341</v>
       </c>
       <c r="F84" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G84" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B85" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D85" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E85" s="7">
         <v>15507</v>
       </c>
       <c r="F85" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G85" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B86" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C86" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D86" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E86" s="7">
         <v>17063</v>
       </c>
       <c r="F86" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G86" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B87" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C87" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D87" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E87" s="7">
         <v>11243</v>
       </c>
       <c r="F87" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G87" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B88" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C88" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D88" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E88" s="7">
         <v>19792</v>
       </c>
       <c r="F88" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G88" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B89" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C89" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D89" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E89" s="7">
         <v>11243</v>
       </c>
       <c r="F89" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G89" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B90" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C90" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D90" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E90" s="7">
         <v>22992</v>
       </c>
       <c r="F90" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G90" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B91" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C91" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D91" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E91" s="7">
         <v>19039</v>
       </c>
       <c r="F91" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G91" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B92" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C92" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D92" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E92" s="7">
         <v>14009</v>
       </c>
       <c r="F92" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G92" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B93" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C93" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D93" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E93" s="7">
         <v>15045</v>
       </c>
       <c r="F93" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G93" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B94" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C94" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D94" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E94" s="7">
         <v>15856</v>
       </c>
       <c r="F94" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G94" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B95" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C95" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D95" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E95" s="7">
         <v>13752</v>
       </c>
       <c r="F95" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G95" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B96" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C96" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D96" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E96" s="7">
         <v>17323</v>
       </c>
       <c r="F96" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G96" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B97" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C97" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D97" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E97" s="7">
         <v>14676</v>
       </c>
       <c r="F97" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G97" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B98" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C98" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D98" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E98" s="7">
         <v>14566</v>
       </c>
       <c r="F98" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G98" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B99" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C99" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D99" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E99" s="7">
         <v>20556</v>
       </c>
       <c r="F99" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G99" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B100" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C100" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D100" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E100" s="7">
         <v>14676</v>
       </c>
       <c r="F100" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G100" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B101" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C101" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D101" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E101" s="7">
         <v>29012</v>
       </c>
       <c r="F101" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G101" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B102" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C102" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D102" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E102" s="7">
         <v>15856</v>
       </c>
       <c r="F102" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G102" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B103" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C103" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D103" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E103" s="7">
         <v>19039</v>
       </c>
       <c r="F103" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G103" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B104" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C104" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D104" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E104" s="7">
         <v>20737</v>
       </c>
       <c r="F104" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G104" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B105" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C105" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D105" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E105" s="7">
         <v>17323</v>
       </c>
       <c r="F105" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G105" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B106" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C106" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D106" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E106" s="7">
         <v>12952</v>
       </c>
       <c r="F106" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G106" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B107" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C107" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D107" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E107" s="7">
         <v>20899</v>
       </c>
       <c r="F107" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G107" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B108" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C108" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D108" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E108" s="7">
         <v>15276</v>
       </c>
       <c r="F108" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G108" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B109" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C109" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D109" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E109" s="7">
         <v>16425</v>
       </c>
       <c r="F109" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G109" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B110" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C110" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D110" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E110" s="7">
         <v>19776</v>
       </c>
       <c r="F110" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G110" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B111" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C111" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D111" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E111" s="7">
         <v>18686</v>
       </c>
       <c r="F111" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G111" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B112" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C112" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D112" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E112" s="7">
         <v>14664</v>
       </c>
       <c r="F112" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G112" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B113" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C113" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D113" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E113" s="7">
         <v>14651</v>
       </c>
       <c r="F113" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G113" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B114" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C114" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D114" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E114" s="7">
         <v>27126</v>
       </c>
       <c r="F114" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G114" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B115" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D115" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E115" s="7">
         <v>14953</v>
       </c>
       <c r="F115" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G115" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B116" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C116" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D116" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E116" s="7">
         <v>22184</v>
       </c>
       <c r="F116" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G116" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B117" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C117" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D117" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E117" s="7">
         <v>16843</v>
       </c>
       <c r="F117" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G117" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B118" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C118" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D118" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E118" s="7">
         <v>17403</v>
       </c>
       <c r="F118" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G118" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B119" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C119" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D119" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E119" s="7">
         <v>17297</v>
       </c>
       <c r="F119" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G119" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B120" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C120" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D120" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E120" s="7">
         <v>16697</v>
       </c>
       <c r="F120" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G120" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B121" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C121" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D121" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E121" s="7">
         <v>19808</v>
       </c>
       <c r="F121" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G121" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B122" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C122" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D122" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E122" s="7">
         <v>16250</v>
       </c>
       <c r="F122" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G122" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B123" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C123" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D123" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E123" s="7">
         <v>17942</v>
       </c>
       <c r="F123" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G123" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B124" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C124" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D124" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E124" s="7">
         <v>16697</v>
       </c>
       <c r="F124" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G124" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B125" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C125" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D125" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E125" s="7">
         <v>17406</v>
       </c>
       <c r="F125" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G125" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B126" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C126" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D126" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E126" s="7">
         <v>13641</v>
       </c>
       <c r="F126" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G126" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B127" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C127" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D127" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E127" s="7">
         <v>24295</v>
       </c>
       <c r="F127" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G127" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B128" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C128" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D128" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E128" s="7">
         <v>19948</v>
       </c>
       <c r="F128" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G128" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="129" spans="1:7">
       <c r="A129" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B129" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C129" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D129" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E129" s="7">
         <v>17632</v>
       </c>
       <c r="F129" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G129" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B130" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C130" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D130" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E130" s="7">
         <v>17145</v>
       </c>
       <c r="F130" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G130" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B131" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C131" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D131" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E131" s="7">
         <v>28801</v>
       </c>
       <c r="F131" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G131" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B132" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C132" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D132" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E132" s="7">
         <v>15498</v>
       </c>
       <c r="F132" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G132" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B133" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C133" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D133" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E133" s="7">
         <v>20842</v>
       </c>
       <c r="F133" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="G133" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B134" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C134" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D134" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E134" s="7">
         <v>16402</v>
       </c>
       <c r="F134" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G134" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B135" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C135" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D135" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E135" s="7">
         <v>15737</v>
       </c>
       <c r="F135" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G135" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="136" spans="1:7">
       <c r="A136" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B136" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C136" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D136" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E136" s="7">
         <v>16952</v>
       </c>
       <c r="F136" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G136" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="137" spans="1:7">
       <c r="A137" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B137" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C137" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D137" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E137" s="7">
         <v>12599</v>
       </c>
       <c r="F137" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G137" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="138" spans="1:7">
       <c r="A138" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B138" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C138" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D138" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E138" s="7">
         <v>18466</v>
       </c>
       <c r="F138" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G138" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="139" spans="1:7">
       <c r="A139" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B139" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C139" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D139" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E139" s="7">
         <v>17436</v>
       </c>
       <c r="F139" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G139" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="140" spans="1:7">
       <c r="A140" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B140" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C140" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D140" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E140" s="7">
         <v>13340</v>
       </c>
       <c r="F140" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G140" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="141" spans="1:7">
       <c r="A141" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B141" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C141" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D141" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E141" s="7">
         <v>15324</v>
       </c>
       <c r="F141" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G141" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B142" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C142" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D142" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E142" s="7">
         <v>17144</v>
       </c>
       <c r="F142" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G142" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" t="s">
+        <v>423</v>
+      </c>
+      <c r="B143" t="s">
+        <v>424</v>
+      </c>
+      <c r="C143" t="s">
         <v>425</v>
       </c>
-      <c r="B143" t="s">
+      <c r="D143" t="s">
         <v>426</v>
       </c>
-      <c r="C143" t="s">
+      <c r="E143" t="s">
         <v>427</v>
       </c>
-      <c r="D143" t="s">
+      <c r="F143" t="s">
         <v>428</v>
       </c>
-      <c r="E143" t="s">
-        <v>429</v>
-      </c>
-      <c r="F143" t="s">
-        <v>430</v>
-      </c>
       <c r="G143" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="144" spans="1:7">
       <c r="A144" t="s">
+        <v>429</v>
+      </c>
+      <c r="B144" t="s">
+        <v>430</v>
+      </c>
+      <c r="C144" t="s">
         <v>431</v>
       </c>
-      <c r="B144" t="s">
+      <c r="D144" t="s">
         <v>432</v>
       </c>
-      <c r="C144" t="s">
+      <c r="E144" t="s">
         <v>433</v>
       </c>
-      <c r="D144" t="s">
+      <c r="F144" t="s">
         <v>434</v>
       </c>
-      <c r="E144" t="s">
-        <v>435</v>
-      </c>
-      <c r="F144" t="s">
-        <v>436</v>
-      </c>
       <c r="G144" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="145" spans="1:7">
       <c r="A145" t="s">
+        <v>435</v>
+      </c>
+      <c r="B145" t="s">
+        <v>436</v>
+      </c>
+      <c r="C145" t="s">
         <v>437</v>
       </c>
-      <c r="B145" t="s">
+      <c r="D145" t="s">
         <v>438</v>
-      </c>
-      <c r="C145" t="s">
-        <v>439</v>
-      </c>
-      <c r="D145" t="s">
-        <v>440</v>
       </c>
       <c r="E145" s="6">
         <v>13671</v>
       </c>
       <c r="F145" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G145" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="146" spans="1:7">
       <c r="A146" t="s">
+        <v>440</v>
+      </c>
+      <c r="B146" t="s">
+        <v>441</v>
+      </c>
+      <c r="C146" t="s">
         <v>442</v>
       </c>
-      <c r="B146" t="s">
+      <c r="D146" t="s">
         <v>443</v>
       </c>
-      <c r="C146" t="s">
+      <c r="E146" t="s">
         <v>444</v>
       </c>
-      <c r="D146" t="s">
+      <c r="F146" t="s">
         <v>445</v>
       </c>
-      <c r="E146" t="s">
-        <v>446</v>
-      </c>
-      <c r="F146" t="s">
-        <v>447</v>
-      </c>
       <c r="G146" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="147" spans="1:7">
       <c r="A147" t="s">
+        <v>446</v>
+      </c>
+      <c r="B147" t="s">
+        <v>447</v>
+      </c>
+      <c r="C147" t="s">
         <v>448</v>
       </c>
-      <c r="B147" t="s">
+      <c r="D147" t="s">
         <v>449</v>
       </c>
-      <c r="C147" t="s">
-        <v>450</v>
-      </c>
-      <c r="D147" t="s">
-        <v>451</v>
-      </c>
       <c r="E147" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F147" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G147" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="148" spans="1:7">
       <c r="A148" t="s">
+        <v>450</v>
+      </c>
+      <c r="B148" t="s">
+        <v>451</v>
+      </c>
+      <c r="C148" t="s">
         <v>452</v>
       </c>
-      <c r="B148" t="s">
+      <c r="D148" t="s">
         <v>453</v>
       </c>
-      <c r="C148" t="s">
+      <c r="E148" t="s">
+        <v>262</v>
+      </c>
+      <c r="F148" t="s">
+        <v>263</v>
+      </c>
+      <c r="G148" t="s">
         <v>454</v>
-      </c>
-      <c r="D148" t="s">
-        <v>455</v>
-      </c>
-      <c r="E148" t="s">
-        <v>264</v>
-      </c>
-      <c r="F148" t="s">
-        <v>265</v>
-      </c>
-      <c r="G148" t="s">
-        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
issue exception driver is null
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prod_tms\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CAF3B7-4DD6-492A-8740-D7BE804BD1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8128ECF-9DCD-4BBA-B2FA-993B7ABC61EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="758">
   <si>
     <t>id</t>
   </si>
@@ -2300,19 +2300,7 @@
     <t>PGX</t>
   </si>
   <si>
-    <t>CA-8HQI316G</t>
-  </si>
-  <si>
-    <t>CA-N6QYX7V2</t>
-  </si>
-  <si>
-    <t>CA-99KQDLJN</t>
-  </si>
-  <si>
-    <t>CA-FUJ1K46M</t>
-  </si>
-  <si>
-    <t>CA-8GG7VCCH</t>
+    <t>CA-JRS0KDBT</t>
   </si>
 </sst>
 </file>
@@ -2705,16 +2693,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5703125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.85546875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="23.28515625"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="36.5703125"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7109375"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.140625"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2754,7 +2742,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>
@@ -2803,7 +2791,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="71.7109375"/>
+    <col min="1" max="1" width="71.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2881,12 +2869,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="27.42578125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="38.28515625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.28515625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.0"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.7109375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.85546875"/>
+    <col min="1" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>

<commit_message>
auto update status core
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prod_tms\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prod_tms\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8128ECF-9DCD-4BBA-B2FA-993B7ABC61EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84764E3-8BE9-4B54-9224-8B8810C9CD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="780">
   <si>
     <t>id</t>
   </si>
@@ -2301,6 +2302,839 @@
   </si>
   <si>
     <t>CA-JRS0KDBT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genetics </t>
+  </si>
+  <si>
+    <r>
+      <t>Verify that the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Intake Agent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (MG/PSS) can create </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Draft</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> case</t>
+    </r>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Intake Agent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (MG) can change case from Draft to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>New</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> case</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>PSS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> can change case from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>New</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Pending</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the case is auto changed from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Pending </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Assigned </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Provider </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">successfully when the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">PSS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">makes a call and the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">provider </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>joins the call successfully</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Verify that the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Provider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> can save the section (reqform, icd code, medicare) successfully and change case from</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Assign</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Ready to send</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>PSS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> can change case from</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Ready to Send</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Result Available</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">PSS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">can change case from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Result Available</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Result Sending</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>PSS c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>an change case from Result Sending to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Pending Follow Up</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> and then forward to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Assigned Follow Up</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Verify that the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Provider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> can change case from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Assigned Follow Up</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Completed by Provider</t>
+    </r>
+  </si>
+  <si>
+    <t>TO REJECTED APRROVED (Daily)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the Intake Agent (MG/PSS) can create </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Draft</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> case and then submits the case from Draft to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>New</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>PSS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> can change case from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>New</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Pending</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>PSS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> can change case from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Pending</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Assign</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Provider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> can change case from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Assign</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Denial Approved</t>
+    </r>
+  </si>
+  <si>
+    <t>TO CANCELLED (Daily)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the Intake Agent (MG/PSS) can create </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Draft</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> case and then submits the case from Draft to New</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>PSS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> can change case from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>New</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Pending</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>PSS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> can change case from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Pending</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Cancelled</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Provider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> can change case from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Assign</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Cancelled</t>
+    </r>
+  </si>
+  <si>
+    <t>TO Completed by Provider (Daily)</t>
   </si>
 </sst>
 </file>
@@ -2310,7 +3144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2341,8 +3175,68 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2355,8 +3249,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000080"/>
+        <bgColor rgb="FF000080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC65911"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -2386,11 +3322,145 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2405,9 +3475,87 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2685,16 +3833,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -2775,7 +3923,265 @@
         <v>10010</v>
       </c>
     </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="32" t="s">
+        <v>779</v>
+      </c>
+      <c r="B5" s="33"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1">
+      <c r="A6" s="34" t="s">
+        <v>758</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="11">
+        <v>1</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>759</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="25.5">
+      <c r="A8" s="11">
+        <v>2</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>761</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="11">
+        <v>3</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>762</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="38.25">
+      <c r="A10" s="11">
+        <v>4</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>763</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="38.25">
+      <c r="A11" s="11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>764</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25.5">
+      <c r="A12" s="11">
+        <v>6</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>765</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="25.5">
+      <c r="A13" s="11">
+        <v>7</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>766</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="25.5">
+      <c r="A14" s="11">
+        <v>8</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>767</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="25.5">
+      <c r="A15" s="11">
+        <v>9</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>768</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="21" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="32" t="s">
+        <v>769</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="31" t="s">
+        <v>758</v>
+      </c>
+      <c r="B17" s="35"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:4" ht="25.5">
+      <c r="A18" s="11">
+        <v>1</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="11">
+        <v>2</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>771</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="11">
+        <v>3</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>772</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="25.5">
+      <c r="A21" s="11">
+        <v>4</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>773</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="30" t="s">
+        <v>774</v>
+      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="31" t="s">
+        <v>758</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:4" ht="25.5">
+      <c r="A24" s="11">
+        <v>1</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>775</v>
+      </c>
+      <c r="C24" s="27"/>
+      <c r="D24" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="11">
+        <v>2</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>776</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="25.5">
+      <c r="A26" s="11">
+        <v>3</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>777</v>
+      </c>
+      <c r="C26" s="28"/>
+      <c r="D26" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="25.5">
+      <c r="A27" s="11">
+        <v>4</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>778</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="14" t="s">
+        <v>760</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update core follow pom
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prod_tms\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84764E3-8BE9-4B54-9224-8B8810C9CD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9E6F19-F4C7-4557-9244-8A89697F3C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="786">
   <si>
     <t>id</t>
   </si>
@@ -2301,9 +2300,6 @@
     <t>PGX</t>
   </si>
   <si>
-    <t>CA-JRS0KDBT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Genetics </t>
   </si>
   <si>
@@ -2344,9 +2340,6 @@
       </rPr>
       <t xml:space="preserve"> case</t>
     </r>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
   <si>
     <r>
@@ -3135,6 +3128,30 @@
   </si>
   <si>
     <t>TO Completed by Provider (Daily)</t>
+  </si>
+  <si>
+    <t>CA-3009G51F</t>
+  </si>
+  <si>
+    <t>CA-UH60J55M</t>
+  </si>
+  <si>
+    <t>CA-SZKEDZQE</t>
+  </si>
+  <si>
+    <t>CA-F9IG0QO4</t>
+  </si>
+  <si>
+    <t>CA-62Z3OBNO</t>
+  </si>
+  <si>
+    <t>CA-H4YBUMC9</t>
+  </si>
+  <si>
+    <t>CA-I2AB6Y4C</t>
+  </si>
+  <si>
+    <t>CA-O3SDOHZ9</t>
   </si>
 </sst>
 </file>
@@ -3835,22 +3852,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125"/>
+    <col min="2" max="2" customWidth="true" width="56.28515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5703125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.85546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.28515625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="36.5703125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3890,7 +3907,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>757</v>
+        <v>785</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>
@@ -3925,13 +3942,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="32" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="B5" s="33"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B6" s="34"/>
       <c r="C6" s="10"/>
@@ -3942,112 +3959,94 @@
         <v>1</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C7" s="13"/>
-      <c r="D7" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="25.5">
       <c r="A8" s="11">
         <v>2</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D8" s="14"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="11">
         <v>3</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C9" s="16"/>
-      <c r="D9" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:11" ht="38.25">
       <c r="A10" s="11">
         <v>4</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C10" s="16"/>
-      <c r="D10" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:11" ht="38.25">
       <c r="A11" s="11">
         <v>5</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C11" s="16"/>
-      <c r="D11" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="1:11" ht="25.5">
       <c r="A12" s="11">
         <v>6</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C12" s="18"/>
-      <c r="D12" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="1:11" ht="25.5">
       <c r="A13" s="11">
         <v>7</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C13" s="19"/>
-      <c r="D13" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:11" ht="25.5">
       <c r="A14" s="11">
         <v>8</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C14" s="19"/>
-      <c r="D14" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:11" ht="25.5">
       <c r="A15" s="11">
         <v>9</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C15" s="19"/>
-      <c r="D15" s="21" t="s">
-        <v>760</v>
-      </c>
+      <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="32" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="22"/>
@@ -4055,7 +4054,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="31" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B17" s="35"/>
       <c r="C17" s="24"/>
@@ -4066,52 +4065,44 @@
         <v>1</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C18" s="27"/>
-      <c r="D18" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D18" s="14"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="11">
         <v>2</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C19" s="28"/>
-      <c r="D19" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="11">
         <v>3</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C20" s="28"/>
-      <c r="D20" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4" ht="25.5">
       <c r="A21" s="11">
         <v>4</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C21" s="28"/>
-      <c r="D21" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="30" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="25"/>
@@ -4119,7 +4110,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="31" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B23" s="31"/>
       <c r="C23" s="25"/>
@@ -4130,48 +4121,40 @@
         <v>1</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C24" s="27"/>
-      <c r="D24" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D24" s="14"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="11">
         <v>2</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C25" s="28"/>
-      <c r="D25" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:4" ht="25.5">
       <c r="A26" s="11">
         <v>3</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C26" s="28"/>
-      <c r="D26" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:4" ht="25.5">
       <c r="A27" s="11">
         <v>4</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C27" s="28"/>
-      <c r="D27" s="14" t="s">
-        <v>760</v>
-      </c>
+      <c r="D27" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4197,7 +4180,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="71.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4275,12 +4258,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="27.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="38.28515625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.28515625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.7109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>

<commit_message>
udpate core for 8 days genetics
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="805">
   <si>
     <t>id</t>
   </si>
@@ -3152,6 +3152,63 @@
   </si>
   <si>
     <t>CA-O3SDOHZ9</t>
+  </si>
+  <si>
+    <t>CA-L92PGNX9</t>
+  </si>
+  <si>
+    <t>CA-TIP1RS3W</t>
+  </si>
+  <si>
+    <t>CA-ZRV6ME9Q</t>
+  </si>
+  <si>
+    <t>CA-Y85V5JEU</t>
+  </si>
+  <si>
+    <t>CA-XKHX9O44</t>
+  </si>
+  <si>
+    <t>CA-EX3N10V4</t>
+  </si>
+  <si>
+    <t>CA-INL2YXAT</t>
+  </si>
+  <si>
+    <t>CA-DB1EO5SN</t>
+  </si>
+  <si>
+    <t>CA-5NWQ80O9</t>
+  </si>
+  <si>
+    <t>CA-8JYC7UDC</t>
+  </si>
+  <si>
+    <t>CA-LMTWPAXZ</t>
+  </si>
+  <si>
+    <t>CA-88Y608YZ</t>
+  </si>
+  <si>
+    <t>CA-1V7RX7HL</t>
+  </si>
+  <si>
+    <t>CA-91DRN25O</t>
+  </si>
+  <si>
+    <t>CA-QQZK5J8R</t>
+  </si>
+  <si>
+    <t>CA-PR1QWY0K</t>
+  </si>
+  <si>
+    <t>CA-9A3P7WPC</t>
+  </si>
+  <si>
+    <t>CA-VYX82KY6</t>
+  </si>
+  <si>
+    <t>CA-FQ5914RW</t>
   </si>
 </sst>
 </file>
@@ -3907,7 +3964,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>785</v>
+        <v>804</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
update pw - flow case
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="962">
   <si>
     <t>id</t>
   </si>
@@ -3263,6 +3263,423 @@
   </si>
   <si>
     <t>CA-5R1LNI1N</t>
+  </si>
+  <si>
+    <t>CA-TASV1NR6</t>
+  </si>
+  <si>
+    <t>CA-I8OGCYRX</t>
+  </si>
+  <si>
+    <t>CA-A8RQMFPC</t>
+  </si>
+  <si>
+    <t>CA-NQIQDDTA</t>
+  </si>
+  <si>
+    <t>CA-82PGKOAJ</t>
+  </si>
+  <si>
+    <t>CA-PNSDO11H</t>
+  </si>
+  <si>
+    <t>CA-7BP5ADYJ</t>
+  </si>
+  <si>
+    <t>CA-R6JEE3A2</t>
+  </si>
+  <si>
+    <t>CA-8BKSRHX9</t>
+  </si>
+  <si>
+    <t>CA-78TDORKI</t>
+  </si>
+  <si>
+    <t>CA-YGSWKQTW</t>
+  </si>
+  <si>
+    <t>CA-5ZD7C3I6</t>
+  </si>
+  <si>
+    <t>CA-BFJK9PPT</t>
+  </si>
+  <si>
+    <t>CA-GVW3F7FF</t>
+  </si>
+  <si>
+    <t>CA-MPHT0GII</t>
+  </si>
+  <si>
+    <t>CA-Y6SUWI3G</t>
+  </si>
+  <si>
+    <t>CA-72F3NZWI</t>
+  </si>
+  <si>
+    <t>CA-K42ULSM9</t>
+  </si>
+  <si>
+    <t>CA-2EXH4BFB</t>
+  </si>
+  <si>
+    <t>CA-1JH59BJH</t>
+  </si>
+  <si>
+    <t>CA-JENZSSVM</t>
+  </si>
+  <si>
+    <t>CA-7B08ITOR</t>
+  </si>
+  <si>
+    <t>CA-07L1AWIV</t>
+  </si>
+  <si>
+    <t>CA-7HVCFXZ0</t>
+  </si>
+  <si>
+    <t>CA-BBKQ9DVV</t>
+  </si>
+  <si>
+    <t>CA-SJVFW7U1</t>
+  </si>
+  <si>
+    <t>CA-5RU0FX6T</t>
+  </si>
+  <si>
+    <t>CA-8BST8V9R</t>
+  </si>
+  <si>
+    <t>CA-ZLF1YCE4</t>
+  </si>
+  <si>
+    <t>CA-2APQ0AOY</t>
+  </si>
+  <si>
+    <t>CA-AVJ38UGA</t>
+  </si>
+  <si>
+    <t>CA-2NZCPMRR</t>
+  </si>
+  <si>
+    <t>CA-CUWP5B32</t>
+  </si>
+  <si>
+    <t>CA-A2SA87A3</t>
+  </si>
+  <si>
+    <t>CA-NA9LXXGO</t>
+  </si>
+  <si>
+    <t>CA-16TGKVZD</t>
+  </si>
+  <si>
+    <t>CA-0K9UG4DI</t>
+  </si>
+  <si>
+    <t>CA-ZKSHOI81</t>
+  </si>
+  <si>
+    <t>CA-HJ7DQZXC</t>
+  </si>
+  <si>
+    <t>CA-6PWLXOI8</t>
+  </si>
+  <si>
+    <t>CA-TIV46Z4U</t>
+  </si>
+  <si>
+    <t>CA-2PXSKYZ5</t>
+  </si>
+  <si>
+    <t>CA-6DS528L2</t>
+  </si>
+  <si>
+    <t>CA-2ZEFWHO5</t>
+  </si>
+  <si>
+    <t>CA-UWKSTQEE</t>
+  </si>
+  <si>
+    <t>CA-A5P7SP4D</t>
+  </si>
+  <si>
+    <t>CA-3CC4TXLE</t>
+  </si>
+  <si>
+    <t>CA-WLYLSGKM</t>
+  </si>
+  <si>
+    <t>CA-74X1B7B8</t>
+  </si>
+  <si>
+    <t>CA-O9R4GSLE</t>
+  </si>
+  <si>
+    <t>CA-Y9USMYFC</t>
+  </si>
+  <si>
+    <t>CA-64I8DYL9</t>
+  </si>
+  <si>
+    <t>CA-175S0SF0</t>
+  </si>
+  <si>
+    <t>CA-54RJH3UP</t>
+  </si>
+  <si>
+    <t>CA-FD4AVQG7</t>
+  </si>
+  <si>
+    <t>CA-OV0M2K52</t>
+  </si>
+  <si>
+    <t>CA-3U69NTZW</t>
+  </si>
+  <si>
+    <t>CA-NR0BMUJI</t>
+  </si>
+  <si>
+    <t>CA-YE2T3JRO</t>
+  </si>
+  <si>
+    <t>CA-X0GHG23S</t>
+  </si>
+  <si>
+    <t>CA-QQ3074ZR</t>
+  </si>
+  <si>
+    <t>CA-XPDYE4ND</t>
+  </si>
+  <si>
+    <t>CA-YKIYCBA9</t>
+  </si>
+  <si>
+    <t>CA-YJ0GI770</t>
+  </si>
+  <si>
+    <t>CA-OEIIY65N</t>
+  </si>
+  <si>
+    <t>CA-RTRPRMV2</t>
+  </si>
+  <si>
+    <t>CA-FYDC7VYP</t>
+  </si>
+  <si>
+    <t>CA-RQM5G5UT</t>
+  </si>
+  <si>
+    <t>CA-NEICLY0W</t>
+  </si>
+  <si>
+    <t>CA-953FUC3O</t>
+  </si>
+  <si>
+    <t>CA-PITUUZZZ</t>
+  </si>
+  <si>
+    <t>CA-FGJD6CS3</t>
+  </si>
+  <si>
+    <t>CA-5IK1IQ6O</t>
+  </si>
+  <si>
+    <t>CA-CG6LC9RN</t>
+  </si>
+  <si>
+    <t>CA-J32C8TM0</t>
+  </si>
+  <si>
+    <t>CA-RGLQ70H5</t>
+  </si>
+  <si>
+    <t>CA-B6PJXQMX</t>
+  </si>
+  <si>
+    <t>CA-XUXBT2W3</t>
+  </si>
+  <si>
+    <t>CA-Q7F8W2RA</t>
+  </si>
+  <si>
+    <t>CA-S3PTK6TV</t>
+  </si>
+  <si>
+    <t>CA-SOARGT8L</t>
+  </si>
+  <si>
+    <t>CA-4OHCQZZK</t>
+  </si>
+  <si>
+    <t>CA-PZ8YBICZ</t>
+  </si>
+  <si>
+    <t>CA-DYITG9EC</t>
+  </si>
+  <si>
+    <t>CA-GDM6WL0T</t>
+  </si>
+  <si>
+    <t>CA-KG1D7PYF</t>
+  </si>
+  <si>
+    <t>CA-QTN7WWVX</t>
+  </si>
+  <si>
+    <t>CA-0JYTVNXG</t>
+  </si>
+  <si>
+    <t>CA-SW28KIJE</t>
+  </si>
+  <si>
+    <t>CA-UTG0UWDV</t>
+  </si>
+  <si>
+    <t>CA-B4FFCSV1</t>
+  </si>
+  <si>
+    <t>CA-ZXZRR91O</t>
+  </si>
+  <si>
+    <t>CA-NRDJTH6E</t>
+  </si>
+  <si>
+    <t>CA-V4LT37NI</t>
+  </si>
+  <si>
+    <t>CA-T943OISK</t>
+  </si>
+  <si>
+    <t>CA-CTA02WAG</t>
+  </si>
+  <si>
+    <t>CA-7YEJYLAI</t>
+  </si>
+  <si>
+    <t>CA-FME24VBE</t>
+  </si>
+  <si>
+    <t>CA-9C2J8AP5</t>
+  </si>
+  <si>
+    <t>CA-CDX9XPCP</t>
+  </si>
+  <si>
+    <t>CA-FAIJZ26G</t>
+  </si>
+  <si>
+    <t>CA-G402XYBI</t>
+  </si>
+  <si>
+    <t>CA-XRL99FCV</t>
+  </si>
+  <si>
+    <t>CA-IOFCX4O3</t>
+  </si>
+  <si>
+    <t>CA-KCC9YW4Z</t>
+  </si>
+  <si>
+    <t>CA-5412TE5K</t>
+  </si>
+  <si>
+    <t>CA-MCLR6T2F</t>
+  </si>
+  <si>
+    <t>CA-X9O253HK</t>
+  </si>
+  <si>
+    <t>CA-WT7GV8H0</t>
+  </si>
+  <si>
+    <t>CA-51NT7JK7</t>
+  </si>
+  <si>
+    <t>CA-933F8G7S</t>
+  </si>
+  <si>
+    <t>CA-F05RC17V</t>
+  </si>
+  <si>
+    <t>CA-PUGUTDOL</t>
+  </si>
+  <si>
+    <t>CA-4LFD19CP</t>
+  </si>
+  <si>
+    <t>CA-1PX40PMK</t>
+  </si>
+  <si>
+    <t>CA-16TJPIRV</t>
+  </si>
+  <si>
+    <t>CA-O8BGXZQX</t>
+  </si>
+  <si>
+    <t>CA-CABW768R</t>
+  </si>
+  <si>
+    <t>CA-GA2TG1H6</t>
+  </si>
+  <si>
+    <t>CA-25S0S22T</t>
+  </si>
+  <si>
+    <t>CA-M61EK49D</t>
+  </si>
+  <si>
+    <t>CA-09PQG4F5</t>
+  </si>
+  <si>
+    <t>CA-GVV8JLL4</t>
+  </si>
+  <si>
+    <t>CA-6A65M5D2</t>
+  </si>
+  <si>
+    <t>CA-CB7CXLCU</t>
+  </si>
+  <si>
+    <t>CA-EEVQS7AK</t>
+  </si>
+  <si>
+    <t>CA-RVUKWNNW</t>
+  </si>
+  <si>
+    <t>CA-76Q22NRL</t>
+  </si>
+  <si>
+    <t>CA-5OIH3PDO</t>
+  </si>
+  <si>
+    <t>CA-51LHL0V3</t>
+  </si>
+  <si>
+    <t>CA-MWKIHJCD</t>
+  </si>
+  <si>
+    <t>CA-6F5TQ3GU</t>
+  </si>
+  <si>
+    <t>CA-HA9JBTVY</t>
+  </si>
+  <si>
+    <t>CA-BD7DQDXL</t>
+  </si>
+  <si>
+    <t>CA-Y9YW1SYC</t>
+  </si>
+  <si>
+    <t>CA-F0AFZJQ4</t>
+  </si>
+  <si>
+    <t>CA-5T18OZAF</t>
+  </si>
+  <si>
+    <t>CA-KFP8T54L</t>
+  </si>
+  <si>
+    <t>CA-YN7BU4AP</t>
   </si>
 </sst>
 </file>
@@ -4025,7 +4442,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>822</v>
+        <v>961</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>776</v>

</xml_diff>

<commit_message>
update run test daily
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="1056">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2388" uniqueCount="1073">
   <si>
     <t>id</t>
   </si>
@@ -3962,6 +3962,57 @@
   </si>
   <si>
     <t>CA-9M7LANMF</t>
+  </si>
+  <si>
+    <t>CA-EXU260R3</t>
+  </si>
+  <si>
+    <t>CA-OOOPHYUX</t>
+  </si>
+  <si>
+    <t>CA-X68EJ6TF</t>
+  </si>
+  <si>
+    <t>CA-P70M5UU5</t>
+  </si>
+  <si>
+    <t>CA-6774RFIT</t>
+  </si>
+  <si>
+    <t>CA-R49KF48L</t>
+  </si>
+  <si>
+    <t>CA-WCLLF59G</t>
+  </si>
+  <si>
+    <t>CA-G7LTHALS</t>
+  </si>
+  <si>
+    <t>CA-GRD4XNW3</t>
+  </si>
+  <si>
+    <t>CA-BNTHHWVZ</t>
+  </si>
+  <si>
+    <t>CA-LPLSUEMC</t>
+  </si>
+  <si>
+    <t>CA-YN3SHCNU</t>
+  </si>
+  <si>
+    <t>CA-844PJOTD</t>
+  </si>
+  <si>
+    <t>CA-RMBY5LMV</t>
+  </si>
+  <si>
+    <t>CA-Y5ULA5AJ</t>
+  </si>
+  <si>
+    <t>CA-UJQGWCNR</t>
+  </si>
+  <si>
+    <t>CA-5NMU9XES</t>
   </si>
 </sst>
 </file>
@@ -4724,7 +4775,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>1055</v>
+        <v>1072</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>776</v>

</xml_diff>